<commit_message>
- adjusted the `CHEN2021` slightly to conform to parent database template
</commit_message>
<xml_diff>
--- a/Chen2021_LowMeltingPointHEAs.xlsx
+++ b/Chen2021_LowMeltingPointHEAs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1029090B-03D6-5147-9A05-12D1318A8D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D9DA5C-9201-F448-8485-E380B348DEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="145">
   <si>
     <t>Metadata</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>ak@psu.edu</t>
-  </si>
-  <si>
-    <t>Direct:</t>
   </si>
   <si>
     <t>HandFetched:</t>
@@ -556,6 +553,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Parent Database:</t>
+  </si>
+  <si>
+    <t>CHEN2021</t>
   </si>
 </sst>
 </file>
@@ -1323,6 +1326,57 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1388,57 +1442,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1748,12 +1751,12 @@
   <dimension ref="A1:T427"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="47" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" style="48" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
@@ -1797,21 +1800,21 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="61"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="78"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1822,25 +1825,25 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="65"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="82"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1856,216 +1859,216 @@
     </row>
     <row r="5" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="66" t="s">
+      <c r="D5" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="E5" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="F5" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="G5" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="H5" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="I5" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="71" t="s">
+      <c r="J5" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="73" t="s">
+      <c r="K5" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="L5" s="85" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="68" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="68" t="s">
+      <c r="N5" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="68" t="s">
+      <c r="O5" s="53" t="s">
         <v>18</v>
-      </c>
-      <c r="O5" s="75" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="76"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="54"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="F7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="G7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="H7" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>29</v>
       </c>
       <c r="I7" s="19">
         <v>298</v>
       </c>
       <c r="J7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="L7" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L7" s="18" t="s">
+      <c r="M7" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="N7" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="N7" s="18" t="s">
+      <c r="O7" s="55"/>
+      <c r="P7" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="77"/>
-      <c r="P7" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q7" s="22" t="s">
+      <c r="R7" s="23" t="s">
         <v>35</v>
-      </c>
-      <c r="R7" s="23" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81" t="s">
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="86" t="s">
+      <c r="N8" s="65"/>
+      <c r="O8" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="87"/>
-      <c r="O8" s="25" t="s">
+      <c r="P8" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="P8" s="88" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="90"/>
-      <c r="S8" s="90"/>
-      <c r="T8" s="91"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="69"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="D9" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="E9" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="F9" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="G9" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="H9" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="I9" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="J9" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="J9" s="33" t="s">
+      <c r="K9" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="L9" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="L9" s="34" t="s">
+      <c r="M9" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="35" t="s">
+      <c r="N9" s="36" t="s">
         <v>54</v>
-      </c>
-      <c r="N9" s="36" t="s">
-        <v>55</v>
       </c>
       <c r="O9" s="37"/>
       <c r="P9" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="Q9" s="39" t="s">
+      <c r="R9" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="R9" s="40" t="s">
+      <c r="S9" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="S9" s="40" t="s">
+      <c r="T9" s="41" t="s">
         <v>59</v>
-      </c>
-      <c r="T9" s="41" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2073,31 +2076,31 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G10" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="42"/>
       <c r="J10" s="43">
-        <f>P10+273.15</f>
+        <f t="shared" ref="J10:J41" si="0">P10+273.15</f>
         <v>283.84999999999997</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O10" s="44"/>
       <c r="P10">
@@ -2109,31 +2112,31 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G11" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="42"/>
       <c r="J11" s="43">
-        <f>P11+273.15</f>
+        <f t="shared" si="0"/>
         <v>284.14999999999998</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O11" s="45"/>
       <c r="P11">
@@ -2145,31 +2148,31 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G12" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H12" s="2"/>
       <c r="J12" s="43">
-        <f>P12+273.15</f>
+        <f t="shared" si="0"/>
         <v>291.95</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O12" s="44"/>
       <c r="P12">
@@ -2181,31 +2184,31 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G13" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H13" s="2"/>
       <c r="J13" s="43">
-        <f>P13+273.15</f>
+        <f t="shared" si="0"/>
         <v>293.7</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O13" s="44"/>
       <c r="P13">
@@ -2217,31 +2220,31 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G14" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H14" s="2"/>
       <c r="J14" s="43">
-        <f>P14+273.15</f>
+        <f t="shared" si="0"/>
         <v>297.75</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P14">
         <v>24.6</v>
@@ -2253,31 +2256,31 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G15" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H15" s="42"/>
       <c r="J15" s="43">
-        <f>P15+273.15</f>
+        <f t="shared" si="0"/>
         <v>298.14999999999998</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P15">
         <v>25</v>
@@ -2288,31 +2291,31 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G16" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H16" s="42"/>
       <c r="J16" s="43">
-        <f>P16+273.15</f>
+        <f t="shared" si="0"/>
         <v>313.14999999999998</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P16">
         <v>40</v>
@@ -2323,31 +2326,31 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G17" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H17" s="42"/>
       <c r="J17" s="43">
-        <f>P17+273.15</f>
+        <f t="shared" si="0"/>
         <v>332.88</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P17">
         <v>59.73</v>
@@ -2358,31 +2361,31 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G18" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H18" s="42"/>
       <c r="J18" s="43">
-        <f>P18+273.15</f>
+        <f t="shared" si="0"/>
         <v>333.15</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P18">
         <v>60</v>
@@ -2393,31 +2396,31 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G19" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H19" s="42"/>
       <c r="J19" s="43">
-        <f>P19+273.15</f>
+        <f t="shared" si="0"/>
         <v>333.15</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P19">
         <v>60</v>
@@ -2428,31 +2431,31 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G20" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H20" s="42"/>
       <c r="J20" s="43">
-        <f>P20+273.15</f>
+        <f t="shared" si="0"/>
         <v>341.15</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P20">
         <v>68</v>
@@ -2463,31 +2466,31 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G21" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H21" s="42"/>
       <c r="J21" s="43">
-        <f>P21+273.15</f>
+        <f t="shared" si="0"/>
         <v>342.15</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P21">
         <v>69</v>
@@ -2498,31 +2501,31 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G22" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H22" s="42"/>
       <c r="J22" s="43">
-        <f>P22+273.15</f>
+        <f t="shared" si="0"/>
         <v>345.15</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P22">
         <v>72</v>
@@ -2533,31 +2536,31 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G23" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H23" s="42"/>
       <c r="J23" s="43">
-        <f>P23+273.15</f>
+        <f t="shared" si="0"/>
         <v>345.15</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P23">
         <v>72</v>
@@ -2568,31 +2571,31 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G24" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H24" s="42"/>
       <c r="J24" s="43">
-        <f>P24+273.15</f>
+        <f t="shared" si="0"/>
         <v>345.28999999999996</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P24">
         <v>72.14</v>
@@ -2603,31 +2606,31 @@
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G25" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H25" s="42"/>
       <c r="J25" s="43">
-        <f>P25+273.15</f>
+        <f t="shared" si="0"/>
         <v>348.15</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P25">
         <v>75</v>
@@ -2638,31 +2641,31 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G26" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H26" s="42"/>
       <c r="J26" s="43">
-        <f>P26+273.15</f>
+        <f t="shared" si="0"/>
         <v>353.84999999999997</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P26">
         <v>80.7</v>
@@ -2673,31 +2676,31 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G27" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H27" s="42"/>
       <c r="J27" s="43">
-        <f>P27+273.15</f>
+        <f t="shared" si="0"/>
         <v>354.15</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P27">
         <v>81</v>
@@ -2708,31 +2711,31 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G28" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H28" s="42"/>
       <c r="J28" s="43">
-        <f>P28+273.15</f>
+        <f t="shared" si="0"/>
         <v>355.15</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M28" s="9"/>
       <c r="N28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P28">
         <v>82</v>
@@ -2743,31 +2746,31 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G29" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H29" s="42"/>
       <c r="J29" s="43">
-        <f>P29+273.15</f>
+        <f t="shared" si="0"/>
         <v>364.15</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P29">
         <v>91</v>
@@ -2778,31 +2781,31 @@
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G30" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H30" s="42"/>
       <c r="J30" s="43">
-        <f>P30+273.15</f>
+        <f t="shared" si="0"/>
         <v>365.15</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P30">
         <v>92</v>
@@ -2813,31 +2816,31 @@
         <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G31" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H31" s="42"/>
       <c r="J31" s="43">
-        <f>P31+273.15</f>
+        <f t="shared" si="0"/>
         <v>366.12</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M31" s="9"/>
       <c r="N31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P31">
         <v>92.97</v>
@@ -2848,31 +2851,31 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G32" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H32" s="42"/>
       <c r="J32" s="43">
-        <f>P32+273.15</f>
+        <f t="shared" si="0"/>
         <v>366.15</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M32" s="9"/>
       <c r="N32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P32">
         <v>93</v>
@@ -2883,31 +2886,31 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G33" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H33" s="42"/>
       <c r="J33" s="43">
-        <f>P33+273.15</f>
+        <f t="shared" si="0"/>
         <v>369.15</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M33" s="9"/>
       <c r="N33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P33">
         <v>96</v>
@@ -2918,31 +2921,31 @@
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G34" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H34" s="42"/>
       <c r="J34" s="43">
-        <f>P34+273.15</f>
+        <f t="shared" si="0"/>
         <v>369.15</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M34" s="9"/>
       <c r="N34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P34">
         <v>96</v>
@@ -2953,31 +2956,31 @@
         <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G35" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H35" s="42"/>
       <c r="J35" s="43">
-        <f>P35+273.15</f>
+        <f t="shared" si="0"/>
         <v>373.15</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M35" s="9"/>
       <c r="N35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P35">
         <v>100</v>
@@ -2988,31 +2991,31 @@
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G36" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H36" s="42"/>
       <c r="J36" s="43">
-        <f>P36+273.15</f>
+        <f t="shared" si="0"/>
         <v>373.15</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M36" s="9"/>
       <c r="N36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P36">
         <v>100</v>
@@ -3023,31 +3026,31 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G37" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H37" s="42"/>
       <c r="J37" s="43">
-        <f>P37+273.15</f>
+        <f t="shared" si="0"/>
         <v>373.15</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M37" s="44"/>
       <c r="N37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P37">
         <v>100</v>
@@ -3058,31 +3061,31 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G38" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H38" s="42"/>
       <c r="J38" s="43">
-        <f>P38+273.15</f>
+        <f t="shared" si="0"/>
         <v>378.15</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M38" s="9"/>
       <c r="N38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P38">
         <v>105</v>
@@ -3093,31 +3096,31 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39" s="42"/>
       <c r="D39" s="42"/>
       <c r="E39" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G39" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H39" s="42"/>
       <c r="J39" s="43">
-        <f>P39+273.15</f>
+        <f t="shared" si="0"/>
         <v>390.15</v>
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M39" s="44"/>
       <c r="N39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P39">
         <v>117</v>
@@ -3128,31 +3131,31 @@
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C40" s="42"/>
       <c r="D40" s="42"/>
       <c r="E40" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G40" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H40" s="42"/>
       <c r="J40" s="43">
-        <f>P40+273.15</f>
+        <f t="shared" si="0"/>
         <v>397.15</v>
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M40" s="44"/>
       <c r="N40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P40">
         <v>124</v>
@@ -3163,31 +3166,31 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" s="42"/>
       <c r="D41" s="42"/>
       <c r="E41" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G41" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H41" s="42"/>
       <c r="J41" s="43">
-        <f>P41+273.15</f>
+        <f t="shared" si="0"/>
         <v>397.15</v>
       </c>
       <c r="K41" s="4"/>
       <c r="L41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M41" s="44"/>
       <c r="N41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P41">
         <v>124</v>
@@ -3198,31 +3201,31 @@
         <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="42"/>
       <c r="E42" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G42" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H42" s="42"/>
       <c r="J42" s="43">
-        <f>P42+273.15</f>
+        <f t="shared" ref="J42:J62" si="1">P42+273.15</f>
         <v>398.45</v>
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M42" s="44"/>
       <c r="N42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P42">
         <v>125.3</v>
@@ -3233,31 +3236,31 @@
         <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C43" s="42"/>
       <c r="D43" s="42"/>
       <c r="E43" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G43" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H43" s="42"/>
       <c r="J43" s="43">
-        <f>P43+273.15</f>
+        <f t="shared" si="1"/>
         <v>405.15</v>
       </c>
       <c r="K43" s="4"/>
       <c r="L43" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M43" s="44"/>
       <c r="N43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P43">
         <v>132</v>
@@ -3268,31 +3271,31 @@
         <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44" s="42"/>
       <c r="D44" s="42"/>
       <c r="E44" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G44" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H44" s="42"/>
       <c r="J44" s="43">
-        <f>P44+273.15</f>
+        <f t="shared" si="1"/>
         <v>411.15</v>
       </c>
       <c r="K44" s="4"/>
       <c r="L44" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M44" s="44"/>
       <c r="N44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P44">
         <v>138</v>
@@ -3303,31 +3306,31 @@
         <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" s="42"/>
       <c r="D45" s="42"/>
       <c r="E45" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G45" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H45" s="42"/>
       <c r="J45" s="43">
-        <f>P45+273.15</f>
+        <f t="shared" si="1"/>
         <v>412.15</v>
       </c>
       <c r="K45" s="4"/>
       <c r="L45" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M45" s="44"/>
       <c r="N45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P45">
         <v>139</v>
@@ -3338,31 +3341,31 @@
         <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" s="42"/>
       <c r="D46" s="42"/>
       <c r="E46" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G46" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H46" s="42"/>
       <c r="J46" s="43">
-        <f>P46+273.15</f>
+        <f t="shared" si="1"/>
         <v>425.15</v>
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M46" s="44"/>
       <c r="N46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P46">
         <v>152</v>
@@ -3373,31 +3376,31 @@
         <v>41</v>
       </c>
       <c r="B47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C47" s="42"/>
       <c r="D47" s="42"/>
       <c r="E47" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G47" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H47" s="42"/>
       <c r="J47" s="43">
-        <f>P47+273.15</f>
+        <f t="shared" si="1"/>
         <v>437.15</v>
       </c>
       <c r="K47" s="4"/>
       <c r="L47" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M47" s="44"/>
       <c r="N47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P47">
         <v>164</v>
@@ -3408,31 +3411,31 @@
         <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C48" s="42"/>
       <c r="D48" s="42"/>
       <c r="E48" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G48" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H48" s="42"/>
       <c r="J48" s="43">
-        <f>P48+273.15</f>
+        <f t="shared" si="1"/>
         <v>439.15</v>
       </c>
       <c r="K48" s="4"/>
       <c r="L48" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M48" s="44"/>
       <c r="N48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P48">
         <v>166</v>
@@ -3443,31 +3446,31 @@
         <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C49" s="42"/>
       <c r="D49" s="42"/>
       <c r="E49" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G49" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H49" s="42"/>
       <c r="J49" s="43">
-        <f>P49+273.15</f>
+        <f t="shared" si="1"/>
         <v>456.15</v>
       </c>
       <c r="K49" s="4"/>
       <c r="L49" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M49" s="44"/>
       <c r="N49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P49">
         <v>183</v>
@@ -3478,31 +3481,31 @@
         <v>44</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" s="42"/>
       <c r="D50" s="42"/>
       <c r="E50" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G50" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H50" s="42"/>
       <c r="J50" s="43">
-        <f>P50+273.15</f>
+        <f t="shared" si="1"/>
         <v>471.15</v>
       </c>
       <c r="K50" s="4"/>
       <c r="L50" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M50" s="44"/>
       <c r="N50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P50">
         <v>198</v>
@@ -3513,31 +3516,31 @@
         <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C51" s="42"/>
       <c r="D51" s="42"/>
       <c r="E51" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G51" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H51" s="42"/>
       <c r="J51" s="43">
-        <f>P51+273.15</f>
+        <f t="shared" si="1"/>
         <v>293.34999999999997</v>
       </c>
       <c r="K51" s="4"/>
       <c r="L51" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M51" s="44"/>
       <c r="N51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P51">
         <v>20.2</v>
@@ -3548,31 +3551,31 @@
         <v>46</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" s="42"/>
       <c r="D52" s="42"/>
       <c r="E52" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G52" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H52" s="42"/>
       <c r="J52" s="43">
-        <f>P52+273.15</f>
+        <f t="shared" si="1"/>
         <v>321.45</v>
       </c>
       <c r="K52" s="4"/>
       <c r="L52" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M52" s="44"/>
       <c r="N52" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P52">
         <v>48.3</v>
@@ -3583,31 +3586,31 @@
         <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" s="42"/>
       <c r="D53" s="42"/>
       <c r="E53" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G53" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H53" s="42"/>
       <c r="J53" s="43">
-        <f>P53+273.15</f>
+        <f t="shared" si="1"/>
         <v>333.57</v>
       </c>
       <c r="K53" s="4"/>
       <c r="L53" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M53" s="44"/>
       <c r="N53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P53">
         <v>60.42</v>
@@ -3618,31 +3621,31 @@
         <v>48</v>
       </c>
       <c r="B54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
       <c r="E54" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G54" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H54" s="42"/>
       <c r="J54" s="43">
-        <f>P54+273.15</f>
+        <f t="shared" si="1"/>
         <v>343.15</v>
       </c>
       <c r="K54" s="4"/>
       <c r="L54" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M54" s="44"/>
       <c r="N54" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P54">
         <v>70</v>
@@ -3653,31 +3656,31 @@
         <v>49</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C55" s="42"/>
       <c r="D55" s="42"/>
       <c r="E55" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G55" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H55" s="42"/>
       <c r="J55" s="43">
-        <f>P55+273.15</f>
+        <f t="shared" si="1"/>
         <v>352.15</v>
       </c>
       <c r="K55" s="4"/>
       <c r="L55" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M55" s="44"/>
       <c r="N55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P55">
         <v>79</v>
@@ -3688,31 +3691,31 @@
         <v>50</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56" s="42"/>
       <c r="D56" s="42"/>
       <c r="E56" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G56" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H56" s="42"/>
       <c r="J56" s="43">
-        <f>P56+273.15</f>
+        <f t="shared" si="1"/>
         <v>373.15</v>
       </c>
       <c r="K56" s="4"/>
       <c r="L56" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M56" s="44"/>
       <c r="N56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P56">
         <v>100</v>
@@ -3723,31 +3726,31 @@
         <v>51</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C57" s="42"/>
       <c r="D57" s="42"/>
       <c r="E57" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G57" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H57" s="42"/>
       <c r="J57" s="43">
-        <f>P57+273.15</f>
+        <f t="shared" si="1"/>
         <v>385.15</v>
       </c>
       <c r="K57" s="4"/>
       <c r="L57" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M57" s="44"/>
       <c r="N57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P57">
         <v>112</v>
@@ -3758,31 +3761,31 @@
         <v>52</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" s="42"/>
       <c r="D58" s="42"/>
       <c r="E58" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G58" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H58" s="42"/>
       <c r="J58" s="43">
-        <f>P58+273.15</f>
+        <f t="shared" si="1"/>
         <v>403.15</v>
       </c>
       <c r="K58" s="4"/>
       <c r="L58" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M58" s="44"/>
       <c r="N58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P58">
         <v>130</v>
@@ -3793,31 +3796,31 @@
         <v>53</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C59" s="42"/>
       <c r="D59" s="42"/>
       <c r="E59" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G59" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H59" s="42"/>
       <c r="J59" s="43">
-        <f>P59+273.15</f>
+        <f t="shared" si="1"/>
         <v>415.15</v>
       </c>
       <c r="K59" s="4"/>
       <c r="L59" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M59" s="44"/>
       <c r="N59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P59">
         <v>142</v>
@@ -3828,31 +3831,31 @@
         <v>54</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" s="42"/>
       <c r="D60" s="42"/>
       <c r="E60" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G60" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H60" s="42"/>
       <c r="J60" s="43">
-        <f>P60+273.15</f>
+        <f t="shared" si="1"/>
         <v>448.15</v>
       </c>
       <c r="K60" s="4"/>
       <c r="L60" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M60" s="44"/>
       <c r="N60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P60">
         <v>175</v>
@@ -3863,31 +3866,31 @@
         <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" s="42"/>
       <c r="D61" s="42"/>
       <c r="E61" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G61" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H61" s="42"/>
       <c r="J61" s="43">
-        <f>P61+273.15</f>
+        <f t="shared" si="1"/>
         <v>454.04999999999995</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M61" s="44"/>
       <c r="N61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P61">
         <v>180.9</v>
@@ -3898,31 +3901,31 @@
         <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C62" s="42"/>
       <c r="D62" s="42"/>
       <c r="E62" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G62" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H62" s="42"/>
       <c r="J62" s="43">
-        <f>P62+273.15</f>
+        <f t="shared" si="1"/>
         <v>473.15</v>
       </c>
       <c r="K62" s="4"/>
       <c r="L62" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M62" s="44"/>
       <c r="N62" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P62">
         <v>200</v>
@@ -3933,33 +3936,33 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
+        <v>140</v>
+      </c>
+      <c r="D63" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D63" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="F63" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G63" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H63" s="42"/>
       <c r="I63" s="3"/>
       <c r="J63" s="43">
-        <f t="shared" ref="J63:J76" si="0">P63+273.15</f>
+        <f t="shared" ref="J63:J76" si="2">P63+273.15</f>
         <v>283.79999999999995</v>
       </c>
       <c r="K63" s="4"/>
       <c r="L63" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M63" s="44"/>
       <c r="N63" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P63">
         <v>10.65</v>
@@ -3970,33 +3973,33 @@
         <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D64" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G64" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H64" s="42"/>
       <c r="I64" s="3"/>
       <c r="J64" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>284.09999999999997</v>
       </c>
       <c r="K64" s="4"/>
       <c r="L64" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M64" s="44"/>
       <c r="N64" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P64">
         <v>10.95</v>
@@ -4007,33 +4010,33 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D65" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G65" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H65" s="42"/>
       <c r="I65" s="3"/>
       <c r="J65" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>288.2</v>
       </c>
       <c r="K65" s="4"/>
       <c r="L65" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M65" s="44"/>
       <c r="N65" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P65">
         <v>15.05</v>
@@ -4044,33 +4047,33 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D66" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G66" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H66" s="42"/>
       <c r="I66" s="3"/>
       <c r="J66" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>293</v>
       </c>
       <c r="K66" s="4"/>
       <c r="L66" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M66" s="44"/>
       <c r="N66" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P66">
         <v>19.850000000000001</v>
@@ -4081,33 +4084,33 @@
         <v>5</v>
       </c>
       <c r="B67" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D67" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G67" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H67" s="42"/>
       <c r="I67" s="3"/>
       <c r="J67" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>293.09999999999997</v>
       </c>
       <c r="K67" s="4"/>
       <c r="L67" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M67" s="44"/>
       <c r="N67" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P67">
         <v>19.95</v>
@@ -4118,33 +4121,33 @@
         <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D68" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G68" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H68" s="42"/>
       <c r="I68" s="3"/>
       <c r="J68" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>327.29999999999995</v>
       </c>
       <c r="K68" s="4"/>
       <c r="L68" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M68" s="44"/>
       <c r="N68" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P68">
         <v>54.15</v>
@@ -4155,33 +4158,33 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D69" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G69" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H69" s="42"/>
       <c r="I69" s="3"/>
       <c r="J69" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>331.5</v>
       </c>
       <c r="K69" s="4"/>
       <c r="L69" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M69" s="44"/>
       <c r="N69" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P69">
         <v>58.35</v>
@@ -4192,33 +4195,33 @@
         <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D70" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G70" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H70" s="42"/>
       <c r="I70" s="3"/>
       <c r="J70" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>334.59999999999997</v>
       </c>
       <c r="K70" s="4"/>
       <c r="L70" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M70" s="44"/>
       <c r="N70" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P70">
         <v>61.45</v>
@@ -4229,33 +4232,33 @@
         <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D71" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G71" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H71" s="42"/>
       <c r="I71" s="3"/>
       <c r="J71" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>344.9</v>
       </c>
       <c r="K71" s="4"/>
       <c r="L71" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M71" s="44"/>
       <c r="N71" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P71">
         <v>71.75</v>
@@ -4266,33 +4269,33 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D72" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G72" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H72" s="42"/>
       <c r="I72" s="3"/>
       <c r="J72" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>346.29999999999995</v>
       </c>
       <c r="K72" s="4"/>
       <c r="L72" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M72" s="44"/>
       <c r="N72" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P72">
         <v>73.150000000000006</v>
@@ -4303,33 +4306,33 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D73" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G73" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H73" s="42"/>
       <c r="I73" s="3"/>
       <c r="J73" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>348.2</v>
       </c>
       <c r="K73" s="4"/>
       <c r="L73" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M73" s="44"/>
       <c r="N73" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P73">
         <v>75.05</v>
@@ -4340,33 +4343,33 @@
         <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D74" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G74" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H74" s="42"/>
       <c r="I74" s="3"/>
       <c r="J74" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>348.9</v>
       </c>
       <c r="K74" s="4"/>
       <c r="L74" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M74" s="44"/>
       <c r="N74" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P74">
         <v>75.75</v>
@@ -4377,33 +4380,33 @@
         <v>13</v>
       </c>
       <c r="B75" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D75" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G75" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H75" s="42"/>
       <c r="I75" s="3"/>
       <c r="J75" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>352.4</v>
       </c>
       <c r="K75" s="4"/>
       <c r="L75" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M75" s="44"/>
       <c r="N75" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P75">
         <v>79.25</v>
@@ -4414,33 +4417,33 @@
         <v>14</v>
       </c>
       <c r="B76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D76" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G76" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H76" s="42"/>
       <c r="I76" s="3"/>
       <c r="J76" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>368.09999999999997</v>
       </c>
       <c r="K76" s="4"/>
       <c r="L76" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M76" s="44"/>
       <c r="N76" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P76">
         <v>94.95</v>
@@ -9715,11 +9718,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -9734,6 +9732,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>